<commit_message>
Got the answers of the notes
</commit_message>
<xml_diff>
--- a/Модуль В/words_count.xlsx
+++ b/Модуль В/words_count.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B694"/>
+  <dimension ref="A1:B963"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,7 +460,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>126</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5">
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12">
@@ -540,7 +540,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>76</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13">
@@ -550,7 +550,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14">
@@ -570,7 +570,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16">
@@ -590,7 +590,7 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -600,7 +600,7 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24">
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="25">
@@ -670,7 +670,7 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26">
@@ -700,7 +700,7 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29">
@@ -760,7 +760,7 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35">
@@ -800,7 +800,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>44</v>
+        <v>54</v>
       </c>
     </row>
     <row r="39">
@@ -840,7 +840,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
@@ -880,7 +880,7 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="47">
@@ -950,7 +950,7 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="54">
@@ -970,7 +970,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56">
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="B62" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63">
@@ -1140,7 +1140,7 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="73">
@@ -1180,7 +1180,7 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="77">
@@ -1190,7 +1190,7 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="78">
@@ -1240,7 +1240,7 @@
         </is>
       </c>
       <c r="B82" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="83">
@@ -1280,7 +1280,7 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="87">
@@ -1340,7 +1340,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="93">
@@ -1350,7 +1350,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="94">
@@ -1360,7 +1360,7 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="95">
@@ -1370,7 +1370,7 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96">
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>14</v>
+        <v>24</v>
       </c>
     </row>
     <row r="97">
@@ -1400,7 +1400,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="99">
@@ -1420,7 +1420,7 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="101">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="102">
@@ -1440,7 +1440,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="103">
@@ -1580,7 +1580,7 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="117">
@@ -1590,7 +1590,7 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>34</v>
+        <v>54</v>
       </c>
     </row>
     <row r="118">
@@ -1600,7 +1600,7 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="119">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="B127" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="128">
@@ -1880,7 +1880,7 @@
         </is>
       </c>
       <c r="B146" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147">
@@ -1910,7 +1910,7 @@
         </is>
       </c>
       <c r="B149" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="150">
@@ -1920,7 +1920,7 @@
         </is>
       </c>
       <c r="B150" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151">
@@ -1940,7 +1940,7 @@
         </is>
       </c>
       <c r="B152" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="153">
@@ -1990,7 +1990,7 @@
         </is>
       </c>
       <c r="B157" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
     <row r="158">
@@ -2110,7 +2110,7 @@
         </is>
       </c>
       <c r="B169" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170">
@@ -2120,7 +2120,7 @@
         </is>
       </c>
       <c r="B170" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="171">
@@ -2170,7 +2170,7 @@
         </is>
       </c>
       <c r="B175" t="n">
-        <v>32</v>
+        <v>68</v>
       </c>
     </row>
     <row r="176">
@@ -2180,7 +2180,7 @@
         </is>
       </c>
       <c r="B176" t="n">
-        <v>22</v>
+        <v>44</v>
       </c>
     </row>
     <row r="177">
@@ -2190,7 +2190,7 @@
         </is>
       </c>
       <c r="B177" t="n">
-        <v>90</v>
+        <v>140</v>
       </c>
     </row>
     <row r="178">
@@ -2200,7 +2200,7 @@
         </is>
       </c>
       <c r="B178" t="n">
-        <v>96</v>
+        <v>134</v>
       </c>
     </row>
     <row r="179">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="B179" t="n">
-        <v>22</v>
+        <v>46</v>
       </c>
     </row>
     <row r="180">
@@ -2230,7 +2230,7 @@
         </is>
       </c>
       <c r="B181" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="182">
@@ -2240,7 +2240,7 @@
         </is>
       </c>
       <c r="B182" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="183">
@@ -2260,7 +2260,7 @@
         </is>
       </c>
       <c r="B184" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="185">
@@ -2280,7 +2280,7 @@
         </is>
       </c>
       <c r="B186" t="n">
-        <v>42</v>
+        <v>80</v>
       </c>
     </row>
     <row r="187">
@@ -2320,7 +2320,7 @@
         </is>
       </c>
       <c r="B190" t="n">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="191">
@@ -2440,7 +2440,7 @@
         </is>
       </c>
       <c r="B202" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="203">
@@ -2450,7 +2450,7 @@
         </is>
       </c>
       <c r="B203" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="B205" t="n">
-        <v>14</v>
+        <v>22</v>
       </c>
     </row>
     <row r="206">
@@ -2640,7 +2640,7 @@
         </is>
       </c>
       <c r="B222" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="223">
@@ -2700,7 +2700,7 @@
         </is>
       </c>
       <c r="B228" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="229">
@@ -2710,7 +2710,7 @@
         </is>
       </c>
       <c r="B229" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="230">
@@ -2740,7 +2740,7 @@
         </is>
       </c>
       <c r="B232" t="n">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="233">
@@ -2750,7 +2750,7 @@
         </is>
       </c>
       <c r="B233" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="234">
@@ -2770,7 +2770,7 @@
         </is>
       </c>
       <c r="B235" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="236">
@@ -2810,7 +2810,7 @@
         </is>
       </c>
       <c r="B239" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240">
@@ -2830,7 +2830,7 @@
         </is>
       </c>
       <c r="B241" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="242">
@@ -2850,7 +2850,7 @@
         </is>
       </c>
       <c r="B243" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="244">
@@ -2880,7 +2880,7 @@
         </is>
       </c>
       <c r="B246" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="247">
@@ -2900,7 +2900,7 @@
         </is>
       </c>
       <c r="B248" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="249">
@@ -2970,7 +2970,7 @@
         </is>
       </c>
       <c r="B255" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="256">
@@ -2980,7 +2980,7 @@
         </is>
       </c>
       <c r="B256" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="257">
@@ -2990,7 +2990,7 @@
         </is>
       </c>
       <c r="B257" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="258">
@@ -3020,7 +3020,7 @@
         </is>
       </c>
       <c r="B260" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="261">
@@ -3040,7 +3040,7 @@
         </is>
       </c>
       <c r="B262" t="n">
-        <v>46</v>
+        <v>74</v>
       </c>
     </row>
     <row r="263">
@@ -3050,7 +3050,7 @@
         </is>
       </c>
       <c r="B263" t="n">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="264">
@@ -3070,7 +3070,7 @@
         </is>
       </c>
       <c r="B265" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="266">
@@ -3090,7 +3090,7 @@
         </is>
       </c>
       <c r="B267" t="n">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="268">
@@ -3110,7 +3110,7 @@
         </is>
       </c>
       <c r="B269" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="270">
@@ -3140,7 +3140,7 @@
         </is>
       </c>
       <c r="B272" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="273">
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="B273" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="274">
@@ -3160,7 +3160,7 @@
         </is>
       </c>
       <c r="B274" t="n">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="275">
@@ -3180,7 +3180,7 @@
         </is>
       </c>
       <c r="B276" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
     </row>
     <row r="277">
@@ -3190,7 +3190,7 @@
         </is>
       </c>
       <c r="B277" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="278">
@@ -3200,7 +3200,7 @@
         </is>
       </c>
       <c r="B278" t="n">
-        <v>50</v>
+        <v>76</v>
       </c>
     </row>
     <row r="279">
@@ -3210,7 +3210,7 @@
         </is>
       </c>
       <c r="B279" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="280">
@@ -3240,7 +3240,7 @@
         </is>
       </c>
       <c r="B282" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="283">
@@ -3290,7 +3290,7 @@
         </is>
       </c>
       <c r="B287" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="288">
@@ -3340,7 +3340,7 @@
         </is>
       </c>
       <c r="B292" t="n">
-        <v>74</v>
+        <v>90</v>
       </c>
     </row>
     <row r="293">
@@ -3350,7 +3350,7 @@
         </is>
       </c>
       <c r="B293" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="294">
@@ -3360,7 +3360,7 @@
         </is>
       </c>
       <c r="B294" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="295">
@@ -3390,7 +3390,7 @@
         </is>
       </c>
       <c r="B297" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="298">
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="B300" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="301">
@@ -3430,7 +3430,7 @@
         </is>
       </c>
       <c r="B301" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="302">
@@ -3440,7 +3440,7 @@
         </is>
       </c>
       <c r="B302" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="303">
@@ -3470,7 +3470,7 @@
         </is>
       </c>
       <c r="B305" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="306">
@@ -3500,7 +3500,7 @@
         </is>
       </c>
       <c r="B308" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="309">
@@ -3520,7 +3520,7 @@
         </is>
       </c>
       <c r="B310" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="311">
@@ -3530,7 +3530,7 @@
         </is>
       </c>
       <c r="B311" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="312">
@@ -3540,7 +3540,7 @@
         </is>
       </c>
       <c r="B312" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="313">
@@ -3550,7 +3550,7 @@
         </is>
       </c>
       <c r="B313" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="314">
@@ -3590,7 +3590,7 @@
         </is>
       </c>
       <c r="B317" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="318">
@@ -3600,7 +3600,7 @@
         </is>
       </c>
       <c r="B318" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="319">
@@ -3610,7 +3610,7 @@
         </is>
       </c>
       <c r="B319" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="320">
@@ -3640,7 +3640,7 @@
         </is>
       </c>
       <c r="B322" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="323">
@@ -3660,7 +3660,7 @@
         </is>
       </c>
       <c r="B324" t="n">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="325">
@@ -3680,7 +3680,7 @@
         </is>
       </c>
       <c r="B326" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="327">
@@ -3700,7 +3700,7 @@
         </is>
       </c>
       <c r="B328" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="329">
@@ -3720,7 +3720,7 @@
         </is>
       </c>
       <c r="B330" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="331">
@@ -3770,7 +3770,7 @@
         </is>
       </c>
       <c r="B335" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="336">
@@ -3790,7 +3790,7 @@
         </is>
       </c>
       <c r="B337" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="338">
@@ -3800,7 +3800,7 @@
         </is>
       </c>
       <c r="B338" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
     </row>
     <row r="339">
@@ -3820,7 +3820,7 @@
         </is>
       </c>
       <c r="B340" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="341">
@@ -3850,7 +3850,7 @@
         </is>
       </c>
       <c r="B343" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="344">
@@ -3860,7 +3860,7 @@
         </is>
       </c>
       <c r="B344" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="345">
@@ -3890,7 +3890,7 @@
         </is>
       </c>
       <c r="B347" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="348">
@@ -3920,7 +3920,7 @@
         </is>
       </c>
       <c r="B350" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="351">
@@ -3940,7 +3940,7 @@
         </is>
       </c>
       <c r="B352" t="n">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="353">
@@ -3950,7 +3950,7 @@
         </is>
       </c>
       <c r="B353" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="354">
@@ -3970,7 +3970,7 @@
         </is>
       </c>
       <c r="B355" t="n">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="356">
@@ -3980,7 +3980,7 @@
         </is>
       </c>
       <c r="B356" t="n">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="357">
@@ -4060,7 +4060,7 @@
         </is>
       </c>
       <c r="B364" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="365">
@@ -4080,7 +4080,7 @@
         </is>
       </c>
       <c r="B366" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="367">
@@ -4170,7 +4170,7 @@
         </is>
       </c>
       <c r="B375" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="376">
@@ -4200,7 +4200,7 @@
         </is>
       </c>
       <c r="B378" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="379">
@@ -4230,7 +4230,7 @@
         </is>
       </c>
       <c r="B381" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="382">
@@ -4330,7 +4330,7 @@
         </is>
       </c>
       <c r="B391" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="392">
@@ -4380,7 +4380,7 @@
         </is>
       </c>
       <c r="B396" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="397">
@@ -4460,7 +4460,7 @@
         </is>
       </c>
       <c r="B404" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="405">
@@ -4480,7 +4480,7 @@
         </is>
       </c>
       <c r="B406" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="407">
@@ -4500,7 +4500,7 @@
         </is>
       </c>
       <c r="B408" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="409">
@@ -4520,7 +4520,7 @@
         </is>
       </c>
       <c r="B410" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="411">
@@ -4560,7 +4560,7 @@
         </is>
       </c>
       <c r="B414" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="415">
@@ -4590,7 +4590,7 @@
         </is>
       </c>
       <c r="B417" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="418">
@@ -4600,7 +4600,7 @@
         </is>
       </c>
       <c r="B418" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="419">
@@ -4620,7 +4620,7 @@
         </is>
       </c>
       <c r="B420" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="421">
@@ -4630,7 +4630,7 @@
         </is>
       </c>
       <c r="B421" t="n">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="422">
@@ -4650,7 +4650,7 @@
         </is>
       </c>
       <c r="B423" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="424">
@@ -4670,7 +4670,7 @@
         </is>
       </c>
       <c r="B425" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="426">
@@ -4780,7 +4780,7 @@
         </is>
       </c>
       <c r="B436" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="437">
@@ -4800,7 +4800,7 @@
         </is>
       </c>
       <c r="B438" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="439">
@@ -4890,7 +4890,7 @@
         </is>
       </c>
       <c r="B447" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
     </row>
     <row r="448">
@@ -4910,7 +4910,7 @@
         </is>
       </c>
       <c r="B449" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="450">
@@ -4920,7 +4920,7 @@
         </is>
       </c>
       <c r="B450" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="451">
@@ -4950,7 +4950,7 @@
         </is>
       </c>
       <c r="B453" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="454">
@@ -4960,7 +4960,7 @@
         </is>
       </c>
       <c r="B454" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="455">
@@ -4990,7 +4990,7 @@
         </is>
       </c>
       <c r="B457" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="458">
@@ -5040,7 +5040,7 @@
         </is>
       </c>
       <c r="B462" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="463">
@@ -5050,7 +5050,7 @@
         </is>
       </c>
       <c r="B463" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="464">
@@ -5080,7 +5080,7 @@
         </is>
       </c>
       <c r="B466" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="467">
@@ -5090,7 +5090,7 @@
         </is>
       </c>
       <c r="B467" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="468">
@@ -5120,7 +5120,7 @@
         </is>
       </c>
       <c r="B470" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="471">
@@ -5170,7 +5170,7 @@
         </is>
       </c>
       <c r="B475" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="476">
@@ -5180,7 +5180,7 @@
         </is>
       </c>
       <c r="B476" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="477">
@@ -5190,7 +5190,7 @@
         </is>
       </c>
       <c r="B477" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="478">
@@ -5230,7 +5230,7 @@
         </is>
       </c>
       <c r="B481" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="482">
@@ -5320,7 +5320,7 @@
         </is>
       </c>
       <c r="B490" t="n">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="491">
@@ -5330,7 +5330,7 @@
         </is>
       </c>
       <c r="B491" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="492">
@@ -5350,7 +5350,7 @@
         </is>
       </c>
       <c r="B493" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="494">
@@ -5380,7 +5380,7 @@
         </is>
       </c>
       <c r="B496" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="497">
@@ -5420,7 +5420,7 @@
         </is>
       </c>
       <c r="B500" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="501">
@@ -5460,7 +5460,7 @@
         </is>
       </c>
       <c r="B504" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="505">
@@ -5500,7 +5500,7 @@
         </is>
       </c>
       <c r="B508" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="509">
@@ -5550,7 +5550,7 @@
         </is>
       </c>
       <c r="B513" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="514">
@@ -5570,7 +5570,7 @@
         </is>
       </c>
       <c r="B515" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="516">
@@ -5600,7 +5600,7 @@
         </is>
       </c>
       <c r="B518" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="519">
@@ -5610,7 +5610,7 @@
         </is>
       </c>
       <c r="B519" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="520">
@@ -5640,7 +5640,7 @@
         </is>
       </c>
       <c r="B522" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="523">
@@ -5650,7 +5650,7 @@
         </is>
       </c>
       <c r="B523" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="524">
@@ -5810,7 +5810,7 @@
         </is>
       </c>
       <c r="B539" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="540">
@@ -5820,7 +5820,7 @@
         </is>
       </c>
       <c r="B540" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="541">
@@ -5880,7 +5880,7 @@
         </is>
       </c>
       <c r="B546" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="547">
@@ -5900,7 +5900,7 @@
         </is>
       </c>
       <c r="B548" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="549">
@@ -5910,7 +5910,7 @@
         </is>
       </c>
       <c r="B549" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="550">
@@ -5950,7 +5950,7 @@
         </is>
       </c>
       <c r="B553" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
     </row>
     <row r="554">
@@ -6060,7 +6060,7 @@
         </is>
       </c>
       <c r="B564" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="565">
@@ -6090,7 +6090,7 @@
         </is>
       </c>
       <c r="B567" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="568">
@@ -6100,7 +6100,7 @@
         </is>
       </c>
       <c r="B568" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="569">
@@ -6110,7 +6110,7 @@
         </is>
       </c>
       <c r="B569" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="570">
@@ -6120,7 +6120,7 @@
         </is>
       </c>
       <c r="B570" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="571">
@@ -6250,7 +6250,7 @@
         </is>
       </c>
       <c r="B583" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="584">
@@ -6270,7 +6270,7 @@
         </is>
       </c>
       <c r="B585" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="586">
@@ -6280,7 +6280,7 @@
         </is>
       </c>
       <c r="B586" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="587">
@@ -6290,7 +6290,7 @@
         </is>
       </c>
       <c r="B587" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="588">
@@ -6300,7 +6300,7 @@
         </is>
       </c>
       <c r="B588" t="n">
-        <v>2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="589">
@@ -6440,7 +6440,7 @@
         </is>
       </c>
       <c r="B602" t="n">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="603">
@@ -6500,7 +6500,7 @@
         </is>
       </c>
       <c r="B608" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="609">
@@ -6520,7 +6520,7 @@
         </is>
       </c>
       <c r="B610" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="611">
@@ -6540,7 +6540,7 @@
         </is>
       </c>
       <c r="B612" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="613">
@@ -6560,7 +6560,7 @@
         </is>
       </c>
       <c r="B614" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="615">
@@ -6570,7 +6570,7 @@
         </is>
       </c>
       <c r="B615" t="n">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="616">
@@ -6670,7 +6670,7 @@
         </is>
       </c>
       <c r="B625" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="626">
@@ -6690,7 +6690,7 @@
         </is>
       </c>
       <c r="B627" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="628">
@@ -6710,7 +6710,7 @@
         </is>
       </c>
       <c r="B629" t="n">
-        <v>6</v>
+        <v>22</v>
       </c>
     </row>
     <row r="630">
@@ -6720,7 +6720,7 @@
         </is>
       </c>
       <c r="B630" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="631">
@@ -6730,7 +6730,7 @@
         </is>
       </c>
       <c r="B631" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="632">
@@ -6750,7 +6750,7 @@
         </is>
       </c>
       <c r="B633" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="634">
@@ -6770,7 +6770,7 @@
         </is>
       </c>
       <c r="B635" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="636">
@@ -6790,7 +6790,7 @@
         </is>
       </c>
       <c r="B637" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="638">
@@ -6800,7 +6800,7 @@
         </is>
       </c>
       <c r="B638" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="639">
@@ -6810,7 +6810,7 @@
         </is>
       </c>
       <c r="B639" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="640">
@@ -6820,7 +6820,7 @@
         </is>
       </c>
       <c r="B640" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="641">
@@ -6870,7 +6870,7 @@
         </is>
       </c>
       <c r="B645" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="646">
@@ -6940,7 +6940,7 @@
         </is>
       </c>
       <c r="B652" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="653">
@@ -7010,7 +7010,7 @@
         </is>
       </c>
       <c r="B659" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="660">
@@ -7030,7 +7030,7 @@
         </is>
       </c>
       <c r="B661" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="662">
@@ -7070,7 +7070,7 @@
         </is>
       </c>
       <c r="B665" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="666">
@@ -7080,7 +7080,7 @@
         </is>
       </c>
       <c r="B666" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="667">
@@ -7090,7 +7090,7 @@
         </is>
       </c>
       <c r="B667" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="668">
@@ -7120,7 +7120,7 @@
         </is>
       </c>
       <c r="B670" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="671">
@@ -7130,7 +7130,7 @@
         </is>
       </c>
       <c r="B671" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="672">
@@ -7140,7 +7140,7 @@
         </is>
       </c>
       <c r="B672" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="673">
@@ -7156,11 +7156,11 @@
     <row r="674">
       <c r="A674" t="inlineStr">
         <is>
-          <t>напомнить</t>
+          <t>напомним</t>
         </is>
       </c>
       <c r="B674" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="675">
@@ -7170,7 +7170,7 @@
         </is>
       </c>
       <c r="B675" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="676">
@@ -7200,7 +7200,7 @@
         </is>
       </c>
       <c r="B678" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="679">
@@ -7220,7 +7220,7 @@
         </is>
       </c>
       <c r="B680" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="681">
@@ -7250,7 +7250,7 @@
         </is>
       </c>
       <c r="B683" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="684">
@@ -7330,7 +7330,7 @@
         </is>
       </c>
       <c r="B691" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="692">
@@ -7360,6 +7360,2696 @@
         </is>
       </c>
       <c r="B694" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>топливо</t>
+        </is>
+      </c>
+      <c r="B695" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>отстать</t>
+        </is>
+      </c>
+      <c r="B696" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>бензин</t>
+        </is>
+      </c>
+      <c r="B697" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>дней</t>
+        </is>
+      </c>
+      <c r="B698" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>май</t>
+        </is>
+      </c>
+      <c r="B699" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>нпз</t>
+        </is>
+      </c>
+      <c r="B700" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>нефтебазах</t>
+        </is>
+      </c>
+      <c r="B701" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>предыдущий</t>
+        </is>
+      </c>
+      <c r="B702" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>чуть</t>
+        </is>
+      </c>
+      <c r="B703" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>менее</t>
+        </is>
+      </c>
+      <c r="B704" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>абсолютно</t>
+        </is>
+      </c>
+      <c r="B705" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>нас</t>
+        </is>
+      </c>
+      <c r="B706" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>если</t>
+        </is>
+      </c>
+      <c r="B707" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>сравнить</t>
+        </is>
+      </c>
+      <c r="B708" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>выше</t>
+        </is>
+      </c>
+      <c r="B709" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>видеть</t>
+        </is>
+      </c>
+      <c r="B710" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>вицепремьер</t>
+        </is>
+      </c>
+      <c r="B711" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>новак</t>
+        </is>
+      </c>
+      <c r="B712" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>принять</t>
+        </is>
+      </c>
+      <c r="B713" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>биржа</t>
+        </is>
+      </c>
+      <c r="B714" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>президент</t>
+        </is>
+      </c>
+      <c r="B715" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>владимир</t>
+        </is>
+      </c>
+      <c r="B716" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>путин</t>
+        </is>
+      </c>
+      <c r="B717" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>намерен</t>
+        </is>
+      </c>
+      <c r="B718" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>реализовывать</t>
+        </is>
+      </c>
+      <c r="B719" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>вьетнам</t>
+        </is>
+      </c>
+      <c r="B720" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>сжидить</t>
+        </is>
+      </c>
+      <c r="B721" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>лидер</t>
+        </is>
+      </c>
+      <c r="B722" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>наука</t>
+        </is>
+      </c>
+      <c r="B723" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>росатом</t>
+        </is>
+      </c>
+      <c r="B724" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>подбор</t>
+        </is>
+      </c>
+      <c r="B725" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>персонал</t>
+        </is>
+      </c>
+      <c r="B726" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>прибыть</t>
+        </is>
+      </c>
+      <c r="B727" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>визит</t>
+        </is>
+      </c>
+      <c r="B728" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>пиролиз</t>
+        </is>
+      </c>
+      <c r="B729" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>этилен</t>
+        </is>
+      </c>
+      <c r="B730" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>аналитик</t>
+        </is>
+      </c>
+      <c r="B731" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>работать</t>
+        </is>
+      </c>
+      <c r="B732" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>загрузка</t>
+        </is>
+      </c>
+      <c r="B733" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>война</t>
+        </is>
+      </c>
+      <c r="B734" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>капитал</t>
+        </is>
+      </c>
+      <c r="B735" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>добавляться</t>
+        </is>
+      </c>
+      <c r="B736" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>кнр</t>
+        </is>
+      </c>
+      <c r="B737" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>устареть</t>
+        </is>
+      </c>
+      <c r="B738" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>игорь</t>
+        </is>
+      </c>
+      <c r="B739" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>сечин</t>
+        </is>
+      </c>
+      <c r="B740" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>характер</t>
+        </is>
+      </c>
+      <c r="B741" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>вынуждена</t>
+        </is>
+      </c>
+      <c r="B742" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>мера</t>
+        </is>
+      </c>
+      <c r="B743" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>защита</t>
+        </is>
+      </c>
+      <c r="B744" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>объект</t>
+        </is>
+      </c>
+      <c r="B745" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>дрон</t>
+        </is>
+      </c>
+      <c r="B746" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>попросить</t>
+        </is>
+      </c>
+      <c r="B747" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>ряд</t>
+        </is>
+      </c>
+      <c r="B748" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>надбавка</t>
+        </is>
+      </c>
+      <c r="B749" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>акциз</t>
+        </is>
+      </c>
+      <c r="B750" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>предоставить</t>
+        </is>
+      </c>
+      <c r="B751" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>льгота</t>
+        </is>
+      </c>
+      <c r="B752" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>расход</t>
+        </is>
+      </c>
+      <c r="B753" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>атака</t>
+        </is>
+      </c>
+      <c r="B754" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>беспилотник</t>
+        </is>
+      </c>
+      <c r="B755" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>письмо</t>
+        </is>
+      </c>
+      <c r="B756" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>глава</t>
+        </is>
+      </c>
+      <c r="B757" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>премьерминистру</t>
+        </is>
+      </c>
+      <c r="B758" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>михаил</t>
+        </is>
+      </c>
+      <c r="B759" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>мишустин</t>
+        </is>
+      </c>
+      <c r="B760" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>инвестнадбавки</t>
+        </is>
+      </c>
+      <c r="B761" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>коэффициент</t>
+        </is>
+      </c>
+      <c r="B762" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>формула</t>
+        </is>
+      </c>
+      <c r="B763" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>получать</t>
+        </is>
+      </c>
+      <c r="B764" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>заключить</t>
+        </is>
+      </c>
+      <c r="B765" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>минфин</t>
+        </is>
+      </c>
+      <c r="B766" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>бюджет</t>
+        </is>
+      </c>
+      <c r="B767" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>выплатить</t>
+        </is>
+      </c>
+      <c r="B768" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>господин</t>
+        </is>
+      </c>
+      <c r="B769" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>предусматривать</t>
+        </is>
+      </c>
+      <c r="B770" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>размер</t>
+        </is>
+      </c>
+      <c r="B771" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>случай</t>
+        </is>
+      </c>
+      <c r="B772" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>обнуляется</t>
+        </is>
+      </c>
+      <c r="B773" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>пеня</t>
+        </is>
+      </c>
+      <c r="B774" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>топменеджер</t>
+        </is>
+      </c>
+      <c r="B775" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>мотивировать</t>
+        </is>
+      </c>
+      <c r="B776" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>ускорить</t>
+        </is>
+      </c>
+      <c r="B777" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>влиять</t>
+        </is>
+      </c>
+      <c r="B778" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>отмена</t>
+        </is>
+      </c>
+      <c r="B779" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>норма</t>
+        </is>
+      </c>
+      <c r="B780" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>успеть</t>
+        </is>
+      </c>
+      <c r="B781" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>эффект</t>
+        </is>
+      </c>
+      <c r="B782" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>предупреждать</t>
+        </is>
+      </c>
+      <c r="B783" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>просить</t>
+        </is>
+      </c>
+      <c r="B784" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>кодекс</t>
+        </is>
+      </c>
+      <c r="B785" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>госдума</t>
+        </is>
+      </c>
+      <c r="B786" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>минпромторг</t>
+        </is>
+      </c>
+      <c r="B787" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>нацпроект</t>
+        </is>
+      </c>
+      <c r="B788" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>импортозависимость</t>
+        </is>
+      </c>
+      <c r="B789" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>кадр</t>
+        </is>
+      </c>
+      <c r="B790" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>накануне</t>
+        </is>
+      </c>
+      <c r="B791" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>уфа</t>
+        </is>
+      </c>
+      <c r="B792" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>стартовать</t>
+        </is>
+      </c>
+      <c r="B793" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>форум</t>
+        </is>
+      </c>
+      <c r="B794" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>выставка</t>
+        </is>
+      </c>
+      <c r="B795" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>посвятить</t>
+        </is>
+      </c>
+      <c r="B796" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>приветствовать</t>
+        </is>
+      </c>
+      <c r="B797" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>башкортостан</t>
+        </is>
+      </c>
+      <c r="B798" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>радий</t>
+        </is>
+      </c>
+      <c r="B799" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>хабиров</t>
+        </is>
+      </c>
+      <c r="B800" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>поблагодарить</t>
+        </is>
+      </c>
+      <c r="B801" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>суметь</t>
+        </is>
+      </c>
+      <c r="B802" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>благодарить</t>
+        </is>
+      </c>
+      <c r="B803" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>сбыт</t>
+        </is>
+      </c>
+      <c r="B804" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>сектор</t>
+        </is>
+      </c>
+      <c r="B805" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>демонстрировать</t>
+        </is>
+      </c>
+      <c r="B806" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>хороший</t>
+        </is>
+      </c>
+      <c r="B807" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>подчеркнуть</t>
+        </is>
+      </c>
+      <c r="B808" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>призвать</t>
+        </is>
+      </c>
+      <c r="B809" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>алга</t>
+        </is>
+      </c>
+      <c r="B810" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>решать</t>
+        </is>
+      </c>
+      <c r="B811" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>трудовой</t>
+        </is>
+      </c>
+      <c r="B812" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>безработица</t>
+        </is>
+      </c>
+      <c r="B813" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>давно</t>
+        </is>
+      </c>
+      <c r="B814" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>радовать</t>
+        </is>
+      </c>
+      <c r="B815" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>потому</t>
+        </is>
+      </c>
+      <c r="B816" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>есть</t>
+        </is>
+      </c>
+      <c r="B817" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>рабочий</t>
+        </is>
+      </c>
+      <c r="B818" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>рука</t>
+        </is>
+      </c>
+      <c r="B819" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>над</t>
+        </is>
+      </c>
+      <c r="B820" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>данной</t>
+        </is>
+      </c>
+      <c r="B821" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>учащимися</t>
+        </is>
+      </c>
+      <c r="B822" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>обозначить</t>
+        </is>
+      </c>
+      <c r="B823" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>юрин</t>
+        </is>
+      </c>
+      <c r="B824" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>цена</t>
+        </is>
+      </c>
+      <c r="B825" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>вызвать</t>
+        </is>
+      </c>
+      <c r="B826" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>метанол</t>
+        </is>
+      </c>
+      <c r="B827" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>аммиак</t>
+        </is>
+      </c>
+      <c r="B828" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>шина</t>
+        </is>
+      </c>
+      <c r="B829" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>волокно</t>
+        </is>
+      </c>
+      <c r="B830" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>пигмент</t>
+        </is>
+      </c>
+      <c r="B831" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>краситель</t>
+        </is>
+      </c>
+      <c r="B832" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>сумма</t>
+        </is>
+      </c>
+      <c r="B833" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>передел</t>
+        </is>
+      </c>
+      <c r="B834" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>широкий</t>
+        </is>
+      </c>
+      <c r="B835" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>частность</t>
+        </is>
+      </c>
+      <c r="B836" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>химия</t>
+        </is>
+      </c>
+      <c r="B837" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>зависимый</t>
+        </is>
+      </c>
+      <c r="B838" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>смочь</t>
+        </is>
+      </c>
+      <c r="B839" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>заместить</t>
+        </is>
+      </c>
+      <c r="B840" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>зависеть</t>
+        </is>
+      </c>
+      <c r="B841" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>замминистра</t>
+        </is>
+      </c>
+      <c r="B842" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>изменить</t>
+        </is>
+      </c>
+      <c r="B843" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>призван</t>
+        </is>
+      </c>
+      <c r="B844" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>полимер</t>
+        </is>
+      </c>
+      <c r="B845" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>начальник</t>
+        </is>
+      </c>
+      <c r="B846" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>департамент</t>
+        </is>
+      </c>
+      <c r="B847" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>пао</t>
+        </is>
+      </c>
+      <c r="B848" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>олег</t>
+        </is>
+      </c>
+      <c r="B849" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>аксютин</t>
+        </is>
+      </c>
+      <c r="B850" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>напомнить</t>
+        </is>
+      </c>
+      <c r="B851" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>кластер</t>
+        </is>
+      </c>
+      <c r="B852" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>которым</t>
+        </is>
+      </c>
+      <c r="B853" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>недавно</t>
+        </is>
+      </c>
+      <c r="B854" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>спикер</t>
+        </is>
+      </c>
+      <c r="B855" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>сделать</t>
+        </is>
+      </c>
+      <c r="B856" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>акцент</t>
+        </is>
+      </c>
+      <c r="B857" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>роль</t>
+        </is>
+      </c>
+      <c r="B858" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>нуль</t>
+        </is>
+      </c>
+      <c r="B859" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>химинвест</t>
+        </is>
+      </c>
+      <c r="B860" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>привязать</t>
+        </is>
+      </c>
+      <c r="B861" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>завезти</t>
+        </is>
+      </c>
+      <c r="B862" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>химинвеста</t>
+        </is>
+      </c>
+      <c r="B863" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>салават</t>
+        </is>
+      </c>
+      <c r="B864" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>медицина</t>
+        </is>
+      </c>
+      <c r="B865" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>структура</t>
+        </is>
+      </c>
+      <c r="B866" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>построить</t>
+        </is>
+      </c>
+      <c r="B867" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>метели</t>
+        </is>
+      </c>
+      <c r="B868" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>пермеата</t>
+        </is>
+      </c>
+      <c r="B869" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>кислый</t>
+        </is>
+      </c>
+      <c r="B870" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>степень</t>
+        </is>
+      </c>
+      <c r="B871" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>метелинском</t>
+        </is>
+      </c>
+      <c r="B872" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>каранелга</t>
+        </is>
+      </c>
+      <c r="B873" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>кулканово</t>
+        </is>
+      </c>
+      <c r="B874" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>сесть</t>
+        </is>
+      </c>
+      <c r="B875" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>интэко</t>
+        </is>
+      </c>
+      <c r="B876" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>речь</t>
+        </is>
+      </c>
+      <c r="B877" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>оснастить</t>
+        </is>
+      </c>
+      <c r="B878" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>станок</t>
+        </is>
+      </c>
+      <c r="B879" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>числовой</t>
+        </is>
+      </c>
+      <c r="B880" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>изготавливать</t>
+        </is>
+      </c>
+      <c r="B881" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>деталь</t>
+        </is>
+      </c>
+      <c r="B882" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>взамен</t>
+        </is>
+      </c>
+      <c r="B883" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>открывать</t>
+        </is>
+      </c>
+      <c r="B884" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>страница</t>
+        </is>
+      </c>
+      <c r="B885" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>непростой</t>
+        </is>
+      </c>
+      <c r="B886" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>вести</t>
+        </is>
+      </c>
+      <c r="B887" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>деятельность</t>
+        </is>
+      </c>
+      <c r="B888" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>выдерживать</t>
+        </is>
+      </c>
+      <c r="B889" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>продажа</t>
+        </is>
+      </c>
+      <c r="B890" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>хмао</t>
+        </is>
+      </c>
+      <c r="B891" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>изготовить</t>
+        </is>
+      </c>
+      <c r="B892" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>сорт</t>
+        </is>
+      </c>
+      <c r="B893" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>дать</t>
+        </is>
+      </c>
+      <c r="B894" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>югралан</t>
+        </is>
+      </c>
+      <c r="B895" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>аналог</t>
+        </is>
+      </c>
+      <c r="B896" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>азербайджан</t>
+        </is>
+      </c>
+      <c r="B897" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>завоевать</t>
+        </is>
+      </c>
+      <c r="B898" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>масло</t>
+        </is>
+      </c>
+      <c r="B899" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>линейка</t>
+        </is>
+      </c>
+      <c r="B900" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>основа</t>
+        </is>
+      </c>
+      <c r="B901" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>югралана</t>
+        </is>
+      </c>
+      <c r="B902" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>компаниипроизводителя</t>
+        </is>
+      </c>
+      <c r="B903" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>али</t>
+        </is>
+      </c>
+      <c r="B904" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>новрузов</t>
+        </is>
+      </c>
+      <c r="B905" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>аэропорт</t>
+        </is>
+      </c>
+      <c r="B906" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>путем</t>
+        </is>
+      </c>
+      <c r="B907" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>нафталан</t>
+        </is>
+      </c>
+      <c r="B908" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>сургут</t>
+        </is>
+      </c>
+      <c r="B909" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>нижневартовск</t>
+        </is>
+      </c>
+      <c r="B910" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>путешественник</t>
+        </is>
+      </c>
+      <c r="B911" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>часто</t>
+        </is>
+      </c>
+      <c r="B912" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>летать</t>
+        </is>
+      </c>
+      <c r="B913" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>ктото</t>
+        </is>
+      </c>
+      <c r="B914" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>захотеть</t>
+        </is>
+      </c>
+      <c r="B915" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>привезти</t>
+        </is>
+      </c>
+      <c r="B916" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>подарок</t>
+        </is>
+      </c>
+      <c r="B917" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>память</t>
+        </is>
+      </c>
+      <c r="B918" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>магазин</t>
+        </is>
+      </c>
+      <c r="B919" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>сайт</t>
+        </is>
+      </c>
+      <c r="B920" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>цитировать</t>
+        </is>
+      </c>
+      <c r="B921" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>новрузова</t>
+        </is>
+      </c>
+      <c r="B922" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>кратчайшие</t>
+        </is>
+      </c>
+      <c r="B923" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>отремонтировать</t>
+        </is>
+      </c>
+      <c r="B924" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>повредить</t>
+        </is>
+      </c>
+      <c r="B925" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>ссылка</t>
+        </is>
+      </c>
+      <c r="B926" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>простаивать</t>
+        </is>
+      </c>
+      <c r="B927" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>быстрый</t>
+        </is>
+      </c>
+      <c r="B928" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>уменьшиться</t>
+        </is>
+      </c>
+      <c r="B929" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>отмечать</t>
+        </is>
+      </c>
+      <c r="B930" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>глубина</t>
+        </is>
+      </c>
+      <c r="B931" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>выжимать</t>
+        </is>
+      </c>
+      <c r="B932" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>максимально</t>
+        </is>
+      </c>
+      <c r="B933" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>многом</t>
+        </is>
+      </c>
+      <c r="B934" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>керосин</t>
+        </is>
+      </c>
+      <c r="B935" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>ранний</t>
+        </is>
+      </c>
+      <c r="B936" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>пояснить</t>
+        </is>
+      </c>
+      <c r="B937" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>эффективность</t>
+        </is>
+      </c>
+      <c r="B938" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>онпз</t>
+        </is>
+      </c>
+      <c r="B939" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>содержать</t>
+        </is>
+      </c>
+      <c r="B940" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>составляющую</t>
+        </is>
+      </c>
+      <c r="B941" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>нам</t>
+        </is>
+      </c>
+      <c r="B942" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>окружать</t>
+        </is>
+      </c>
+      <c r="B943" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>барр</t>
+        </is>
+      </c>
+      <c r="B944" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>европа</t>
+        </is>
+      </c>
+      <c r="B945" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>китай</t>
+        </is>
+      </c>
+      <c r="B946" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>пятый</t>
+        </is>
+      </c>
+      <c r="B947" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>угроза</t>
+        </is>
+      </c>
+      <c r="B948" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>проанализировать</t>
+        </is>
+      </c>
+      <c r="B949" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>процента</t>
+        </is>
+      </c>
+      <c r="B950" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>март</t>
+        </is>
+      </c>
+      <c r="B951" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>предыдущей</t>
+        </is>
+      </c>
+      <c r="B952" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>запрет</t>
+        </is>
+      </c>
+      <c r="B953" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>ожидать</t>
+        </is>
+      </c>
+      <c r="B954" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>нефтепереработка</t>
+        </is>
+      </c>
+      <c r="B955" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>прогноз</t>
+        </is>
+      </c>
+      <c r="B956" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>сохраняться</t>
+        </is>
+      </c>
+      <c r="B957" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>близком</t>
+        </is>
+      </c>
+      <c r="B958" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>прайм</t>
+        </is>
+      </c>
+      <c r="B959" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>февраль</t>
+        </is>
+      </c>
+      <c r="B960" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>павел</t>
+        </is>
+      </c>
+      <c r="B961" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>сорокин</t>
+        </is>
+      </c>
+      <c r="B962" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>нарастить</t>
+        </is>
+      </c>
+      <c r="B963" t="n">
         <v>2</v>
       </c>
     </row>

</xml_diff>